<commit_message>
Adds Industry Category subscript to SoCiIEPTtB Share of Change in Industry Expenses Passed Through to Buyers; values set to 1 for all industries
</commit_message>
<xml_diff>
--- a/InputData/indst/SoCiIEPTtB/Shr of Cng in Indst Expenses Passed Thr to Buyers.xlsx
+++ b/InputData/indst/SoCiIEPTtB/Shr of Cng in Indst Expenses Passed Thr to Buyers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\indst\SoCiIEPTtB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\U.S. Models\eps-us\InputData\indst\SoCiIEPTtB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D170B4D2-127F-4FC7-9E13-42171A432FA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D87643-3FBD-4818-AB4B-E532AC1F3B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="915" windowWidth="24090" windowHeight="16245" xr2:uid="{C45C27AA-02D4-49AC-94B3-A048BBC9260E}"/>
+    <workbookView xWindow="35730" yWindow="4035" windowWidth="21600" windowHeight="12525" activeTab="1" xr2:uid="{C45C27AA-02D4-49AC-94B3-A048BBC9260E}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>SoCiIEPTtB Share of Change in Industry Expenses Passed Through to Buyers</t>
   </si>
@@ -138,10 +138,82 @@
     <t>Unit: dimensionless (% passthrough)</t>
   </si>
   <si>
-    <t>Share of expenses</t>
-  </si>
-  <si>
     <t>Paid by consumers</t>
+  </si>
+  <si>
+    <t>agriculture and forestry 01T03</t>
+  </si>
+  <si>
+    <t>coal mining 05</t>
+  </si>
+  <si>
+    <t>oil and gas extraction 06</t>
+  </si>
+  <si>
+    <t>other mining and quarrying 07T08</t>
+  </si>
+  <si>
+    <t>food beverage and tobacco 10T12</t>
+  </si>
+  <si>
+    <t>textiles apparel and leather 13T15</t>
+  </si>
+  <si>
+    <t>wood products 16</t>
+  </si>
+  <si>
+    <t>pulp paper and printing 17T18</t>
+  </si>
+  <si>
+    <t>refined petroleum and coke 19</t>
+  </si>
+  <si>
+    <t>chemicals 20</t>
+  </si>
+  <si>
+    <t>rubber and plastic products 22</t>
+  </si>
+  <si>
+    <t>glass and glass products 231</t>
+  </si>
+  <si>
+    <t>cement and other nonmetallic minerals 239</t>
+  </si>
+  <si>
+    <t>iron and steel 241</t>
+  </si>
+  <si>
+    <t>other metals 242</t>
+  </si>
+  <si>
+    <t>metal products except machinery and vehicles 25</t>
+  </si>
+  <si>
+    <t>computers and electronics 26</t>
+  </si>
+  <si>
+    <t>appliances and electrical equipment 27</t>
+  </si>
+  <si>
+    <t>other machinery 28</t>
+  </si>
+  <si>
+    <t>road vehicles 29</t>
+  </si>
+  <si>
+    <t>nonroad vehicles 30</t>
+  </si>
+  <si>
+    <t>other manufacturing 31T33</t>
+  </si>
+  <si>
+    <t>energy pipelines and gas processing 352T353</t>
+  </si>
+  <si>
+    <t>water and waste 36T39</t>
+  </si>
+  <si>
+    <t>construction 41T43</t>
   </si>
 </sst>
 </file>
@@ -202,14 +274,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -230,9 +301,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -270,7 +341,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -376,7 +447,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -518,7 +589,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -528,19 +599,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA9904B-1EB4-4402-820D-BB1B47048552}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="91.140625" customWidth="1"/>
+    <col min="2" max="2" width="91.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -548,157 +621,157 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1</v>
       </c>
@@ -720,30 +793,248 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
       <c r="B2">
-        <f>About!A42</f>
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25">
+        <f>About!A$42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26">
+        <f>About!A$42</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>